<commit_message>
LCV duzeltmeleri yapildi, HDV ilk model eklendi
</commit_message>
<xml_diff>
--- a/r_input/LCV_HCV inputs.xlsx
+++ b/r_input/LCV_HCV inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519F1C8A-4F70-43EA-BBD6-3D45D98DFC43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F454CBAF-C3E4-4642-870C-B5561D5F797D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E25ACDE5-3E01-46FD-BE83-2A8099FD5975}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E25ACDE5-3E01-46FD-BE83-2A8099FD5975}"/>
   </bookViews>
   <sheets>
     <sheet name="LCV" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>segment</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>kdv</t>
+  </si>
+  <si>
+    <t>net_fiyat</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B7C08D-34A3-4456-96EB-6D841A91B715}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -688,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971154D8-6129-44D7-B9EF-EFA94F119A71}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Turkce karakterler hatalari duzeltildi
</commit_message>
<xml_diff>
--- a/r_input/LCV_HCV inputs.xlsx
+++ b/r_input/LCV_HCV inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C7365-6E14-4C63-B6BB-CDC7274E4498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F459FDC-A12E-4DE4-85BB-8E9CC9CD5E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E25ACDE5-3E01-46FD-BE83-2A8099FD5975}"/>
   </bookViews>
@@ -41,6 +41,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={D1AF7448-A769-47D2-92A2-80D753A32D03}</author>
+    <author>tc={C7C266A8-AD09-4CE9-988F-F77E329EBDBE}</author>
   </authors>
   <commentList>
     <comment ref="K4" authorId="0" shapeId="0" xr:uid="{D1AF7448-A769-47D2-92A2-80D753A32D03}">
@@ -51,6 +52,14 @@
     https://www.carbonindependent.org/20.html#:~:text=the%20average%20passengers%20per%20bus,buses%20is%20822%20g%20%2F%20km</t>
       </text>
     </comment>
+    <comment ref="K9" authorId="1" shapeId="0" xr:uid="{C7C266A8-AD09-4CE9-988F-F77E329EBDBE}">
+      <text>
+        <t>[Yorum yazışması]
+Excel sürümünüz bu yorum yazışmasını okumanıza izin veriyor, ancak dosya daha yeni bir Excel sürümünde açılırsa, yapılan düzenlemeler kaldırılır. Daha fazla bilgi: https://go.microsoft.com/fwlink/?linkid=870924.
+Açıklama:
+    https://www.transportenvironment.org/sites/te/files/publications/2015%2009%20TE%20Briefing%20Truck%20CO2%20Too%20big%20to%20ignore_FINAL.pdf</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -207,7 +216,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +239,12 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -613,6 +628,9 @@
   <threadedComment ref="K4" dT="2020-10-02T03:47:18.56" personId="{E647A31E-5394-4B01-B799-A4CF11830264}" id="{D1AF7448-A769-47D2-92A2-80D753A32D03}">
     <text>https://www.carbonindependent.org/20.html#:~:text=the%20average%20passengers%20per%20bus,buses%20is%20822%20g%20%2F%20km</text>
   </threadedComment>
+  <threadedComment ref="K9" dT="2020-10-04T04:01:50.94" personId="{E647A31E-5394-4B01-B799-A4CF11830264}" id="{C7C266A8-AD09-4CE9-988F-F77E329EBDBE}">
+    <text>https://www.transportenvironment.org/sites/te/files/publications/2015%2009%20TE%20Briefing%20Truck%20CO2%20Too%20big%20to%20ignore_FINAL.pdf</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -621,17 +639,24 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1468,7 +1493,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,7 +1535,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>0.04</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="D3">
         <f>[1]mevcut_degiskenler!$B$2</f>

</xml_diff>